<commit_message>
Complete the scenario "verify that madicine is order from home page after clicking findmy treatment button"
</commit_message>
<xml_diff>
--- a/utils/workbook.xlsx
+++ b/utils/workbook.xlsx
@@ -375,9 +375,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -408,9 +408,23 @@
         <v>OlsonCeledon@yopmail.com</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Matthew</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Davis</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Test@1234</v>
+      </c>
+      <c r="D3" t="str">
+        <v>MatthewDavis@yopmail.com</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Complete order from home page into category details
</commit_message>
<xml_diff>
--- a/utils/workbook.xlsx
+++ b/utils/workbook.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -422,9 +422,37 @@
         <v>MatthewDavis@yopmail.com</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Nathan</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Wagner</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Test@1234</v>
+      </c>
+      <c r="D4" t="str">
+        <v>NathanWagner@yopmail.com</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Reamer</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Schickowski</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Test@1234</v>
+      </c>
+      <c r="D5" t="str">
+        <v>ReamerSchickowski@yopmail.com</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>